<commit_message>
Update documents/ET kalender 18-19 06102018.xlsx
Kalender bijgewerkt
</commit_message>
<xml_diff>
--- a/documents/ET kalender 18-19 06102018.xlsx
+++ b/documents/ET kalender 18-19 06102018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VantageGroningenGit\VantageGroningen\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA643F5-1DFA-436B-8840-40E726D0AB6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311A0E4F-E4E5-47DA-9C6F-A2E6783E52C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{ED6C9CC8-F603-4F8A-90F2-10D78C5C1E86}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="60">
   <si>
     <t>Datum</t>
   </si>
@@ -207,7 +208,10 @@
     <t>FotoFinish</t>
   </si>
   <si>
-    <t>Reitse</t>
+    <t>Floris Klunder</t>
+  </si>
+  <si>
+    <t>Karuud Pots</t>
   </si>
 </sst>
 </file>
@@ -588,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A483D3-646C-4782-A31E-399667822D5C}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,10 +604,11 @@
     <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +627,11 @@
       <c r="F1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43379.666666666664</v>
       </c>
@@ -637,7 +645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43386.666666666664</v>
       </c>
@@ -651,7 +659,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43386.791666666664</v>
       </c>
@@ -665,7 +673,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43393.802083333336</v>
       </c>
@@ -679,7 +687,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43400.666666666664</v>
       </c>
@@ -693,7 +701,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43400.791666666664</v>
       </c>
@@ -707,7 +715,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43407.791666666664</v>
       </c>
@@ -721,7 +729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43414.666666666664</v>
       </c>
@@ -735,7 +743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43421.666666666664</v>
       </c>
@@ -749,7 +757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43428.541666666664</v>
       </c>
@@ -766,7 +774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43428.8125</v>
       </c>
@@ -780,7 +788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>43442.666666666664</v>
       </c>
@@ -794,10 +802,10 @@
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>43443.666666666664</v>
       </c>
@@ -814,7 +822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43449.666666666664</v>
       </c>
@@ -828,7 +836,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43456.791666666664</v>
       </c>
@@ -842,7 +850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43457.770833333336</v>
       </c>
@@ -856,7 +864,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43470.666666666664</v>
       </c>
@@ -870,7 +878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43470.791666666664</v>
       </c>
@@ -884,7 +892,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43477.791666666664</v>
       </c>
@@ -894,11 +902,9 @@
       <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43484.8125</v>
       </c>
@@ -912,7 +918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43491.666666666664</v>
       </c>
@@ -926,7 +932,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43497.708333333336</v>
       </c>
@@ -934,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>48</v>
@@ -945,8 +951,11 @@
       <c r="F23" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43498.541666666664</v>
       </c>
@@ -954,19 +963,20 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="E24" s="7"/>
       <c r="F24" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43499.708333333336</v>
       </c>
@@ -974,7 +984,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>39</v>
@@ -985,8 +995,11 @@
       <c r="F25" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43506.833333333336</v>
       </c>
@@ -997,10 +1010,10 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43519.791666666664</v>
       </c>
@@ -1011,10 +1024,10 @@
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43520.833333333336</v>
       </c>
@@ -1024,11 +1037,9 @@
       <c r="C28" t="s">
         <v>45</v>
       </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43533.666666666664</v>
       </c>
@@ -1036,13 +1047,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43533.791666666664</v>
       </c>
@@ -1052,11 +1063,9 @@
       <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43537.760416666664</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43544.760416666664</v>
       </c>
@@ -1157,14 +1166,14 @@
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>37</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1191,14 +1200,14 @@
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1240,7 +1249,7 @@
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>48</v>
@@ -1256,7 +1265,7 @@
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>41</v>
@@ -1272,7 +1281,7 @@
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
         <v>49</v>
@@ -1288,14 +1297,14 @@
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>